<commit_message>
[Implementation] added Student, StudentList
</commit_message>
<xml_diff>
--- a/Track.xlsx
+++ b/Track.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edwardxc/git/buddySystem/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A0CF5B5-F327-F24E-BF41-6D9E5B7C08B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D08201-736B-474A-9098-79B62352ED89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17120" xr2:uid="{7D8A488B-E589-6340-A98F-33E9BF1CB4C3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="208">
   <si>
     <t xml:space="preserve">LJ Que </t>
   </si>
@@ -656,19 +656,10 @@
     <t>lsorom@bowdoin.edu</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
     <t>Cheng Xing</t>
   </si>
   <si>
     <t>cxing@bowdoin.edu</t>
-  </si>
-  <si>
-    <t>Id</t>
   </si>
 </sst>
 </file>
@@ -1020,10 +1011,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A6CF95-BBA5-3F4C-B82E-A41B70A08D17}">
-  <dimension ref="A1:C105"/>
+  <dimension ref="A1:C104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1032,1261 +1023,1250 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>210</v>
+      <c r="A1">
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>206</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>207</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
+        <f>A1+1</f>
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
       <c r="C2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
-        <f>A2+1</f>
+        <f t="shared" ref="A3:A66" si="0">A2+1</f>
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
       <c r="C3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
-        <f t="shared" ref="A4:A67" si="0">A3+1</f>
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
       <c r="C4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
       <c r="C5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
       <c r="C6" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
       <c r="C7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
       <c r="C8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
       <c r="C9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
       <c r="C10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
       <c r="C11" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
       <c r="C12" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
       <c r="C13" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
-        <v>12</v>
-      </c>
       <c r="C14" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>13</v>
-      </c>
       <c r="C15" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
-        <v>14</v>
-      </c>
       <c r="C16" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
-        <v>15</v>
-      </c>
       <c r="C17" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
-        <v>16</v>
-      </c>
       <c r="C18" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
-        <v>17</v>
-      </c>
       <c r="C19" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
-        <v>18</v>
-      </c>
       <c r="C20" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
-        <v>19</v>
-      </c>
       <c r="C21" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
         <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
-        <v>20</v>
-      </c>
       <c r="C22" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
         <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
-        <v>21</v>
-      </c>
       <c r="C23" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
         <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
-        <v>22</v>
-      </c>
       <c r="C24" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
         <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
-        <v>23</v>
-      </c>
       <c r="C25" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
         <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B26" t="s">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
-        <v>24</v>
-      </c>
       <c r="C26" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
         <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
-        <v>25</v>
-      </c>
       <c r="C27" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
         <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
         <v>27</v>
       </c>
-      <c r="B28" t="s">
-        <v>26</v>
-      </c>
       <c r="C28" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
         <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B29" t="s">
         <v>28</v>
       </c>
-      <c r="B29" t="s">
-        <v>27</v>
-      </c>
       <c r="C29" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
         <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
-        <v>28</v>
-      </c>
       <c r="C30" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
         <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B31" t="s">
         <v>30</v>
       </c>
-      <c r="B31" t="s">
-        <v>29</v>
-      </c>
       <c r="C31" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32">
         <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B32" t="s">
         <v>31</v>
       </c>
-      <c r="B32" t="s">
-        <v>30</v>
-      </c>
       <c r="C32" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33">
         <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B33" t="s">
         <v>32</v>
       </c>
-      <c r="B33" t="s">
-        <v>31</v>
-      </c>
       <c r="C33" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34">
         <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B34" t="s">
         <v>33</v>
       </c>
-      <c r="B34" t="s">
-        <v>32</v>
-      </c>
       <c r="C34" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35">
         <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B35" t="s">
         <v>34</v>
       </c>
-      <c r="B35" t="s">
-        <v>33</v>
-      </c>
       <c r="C35" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36">
         <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B36" t="s">
         <v>35</v>
       </c>
-      <c r="B36" t="s">
-        <v>34</v>
-      </c>
       <c r="C36" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37">
         <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="B37" t="s">
         <v>36</v>
       </c>
-      <c r="B37" t="s">
-        <v>35</v>
-      </c>
       <c r="C37" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38">
         <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="B38" t="s">
         <v>37</v>
       </c>
-      <c r="B38" t="s">
-        <v>36</v>
-      </c>
       <c r="C38" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39">
         <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B39" t="s">
         <v>38</v>
       </c>
-      <c r="B39" t="s">
-        <v>37</v>
-      </c>
       <c r="C39" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40">
         <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B40" t="s">
         <v>39</v>
       </c>
-      <c r="B40" t="s">
-        <v>38</v>
-      </c>
       <c r="C40" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41">
         <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B41" t="s">
         <v>40</v>
       </c>
-      <c r="B41" t="s">
-        <v>39</v>
-      </c>
       <c r="C41" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42">
         <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B42" t="s">
         <v>41</v>
       </c>
-      <c r="B42" t="s">
-        <v>40</v>
-      </c>
       <c r="C42" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43">
         <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="B43" t="s">
         <v>42</v>
       </c>
-      <c r="B43" t="s">
-        <v>41</v>
-      </c>
       <c r="C43" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44">
         <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="B44" t="s">
         <v>43</v>
       </c>
-      <c r="B44" t="s">
-        <v>42</v>
-      </c>
       <c r="C44" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45">
         <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="B45" t="s">
         <v>44</v>
       </c>
-      <c r="B45" t="s">
-        <v>43</v>
-      </c>
       <c r="C45" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46">
         <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="B46" t="s">
         <v>45</v>
       </c>
-      <c r="B46" t="s">
-        <v>44</v>
-      </c>
       <c r="C46" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47">
         <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="B47" t="s">
         <v>46</v>
       </c>
-      <c r="B47" t="s">
-        <v>45</v>
-      </c>
       <c r="C47" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48">
         <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="B48" t="s">
         <v>47</v>
       </c>
-      <c r="B48" t="s">
-        <v>46</v>
-      </c>
       <c r="C48" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49">
         <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="B49" t="s">
         <v>48</v>
       </c>
-      <c r="B49" t="s">
-        <v>47</v>
-      </c>
       <c r="C49" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50">
         <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="B50" t="s">
         <v>49</v>
       </c>
-      <c r="B50" t="s">
-        <v>48</v>
-      </c>
       <c r="C50" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51">
         <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="B51" t="s">
         <v>50</v>
       </c>
-      <c r="B51" t="s">
-        <v>49</v>
-      </c>
       <c r="C51" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52">
         <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="B52" t="s">
         <v>51</v>
       </c>
-      <c r="B52" t="s">
-        <v>50</v>
-      </c>
       <c r="C52" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53">
         <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="B53" t="s">
         <v>52</v>
       </c>
-      <c r="B53" t="s">
-        <v>51</v>
-      </c>
       <c r="C53" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54">
         <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="B54" t="s">
         <v>53</v>
       </c>
-      <c r="B54" t="s">
-        <v>52</v>
-      </c>
       <c r="C54" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55">
         <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="B55" t="s">
         <v>54</v>
       </c>
-      <c r="B55" t="s">
-        <v>53</v>
-      </c>
       <c r="C55" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56">
         <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="B56" t="s">
         <v>55</v>
       </c>
-      <c r="B56" t="s">
-        <v>54</v>
-      </c>
       <c r="C56" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57">
         <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="B57" t="s">
         <v>56</v>
       </c>
-      <c r="B57" t="s">
-        <v>55</v>
-      </c>
       <c r="C57" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58">
         <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="B58" t="s">
         <v>57</v>
       </c>
-      <c r="B58" t="s">
-        <v>56</v>
-      </c>
       <c r="C58" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59">
         <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="B59" t="s">
         <v>58</v>
       </c>
-      <c r="B59" t="s">
-        <v>57</v>
-      </c>
       <c r="C59" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60">
         <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="B60" t="s">
         <v>59</v>
       </c>
-      <c r="B60" t="s">
-        <v>58</v>
-      </c>
       <c r="C60" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61">
         <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="B61" t="s">
         <v>60</v>
       </c>
-      <c r="B61" t="s">
-        <v>59</v>
-      </c>
       <c r="C61" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62">
         <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="B62" t="s">
         <v>61</v>
       </c>
-      <c r="B62" t="s">
-        <v>60</v>
-      </c>
       <c r="C62" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63">
         <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="B63" t="s">
         <v>62</v>
       </c>
-      <c r="B63" t="s">
-        <v>61</v>
-      </c>
       <c r="C63" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64">
         <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="B64" t="s">
         <v>63</v>
       </c>
-      <c r="B64" t="s">
-        <v>62</v>
-      </c>
       <c r="C64" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65">
         <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="B65" t="s">
         <v>64</v>
       </c>
-      <c r="B65" t="s">
-        <v>63</v>
-      </c>
       <c r="C65" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66">
         <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="B66" t="s">
         <v>65</v>
       </c>
-      <c r="B66" t="s">
-        <v>64</v>
-      </c>
       <c r="C66" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A67:A104" si="1">A66+1</f>
+        <v>67</v>
+      </c>
+      <c r="B67" t="s">
         <v>66</v>
       </c>
-      <c r="B67" t="s">
-        <v>65</v>
-      </c>
       <c r="C67" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68">
-        <f t="shared" ref="A68:A105" si="1">A67+1</f>
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+      <c r="B68" t="s">
         <v>67</v>
       </c>
-      <c r="B68" t="s">
-        <v>66</v>
-      </c>
       <c r="C68" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69">
         <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
+      <c r="B69" t="s">
         <v>68</v>
       </c>
-      <c r="B69" t="s">
-        <v>67</v>
-      </c>
       <c r="C69" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70">
         <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="B70" t="s">
         <v>69</v>
       </c>
-      <c r="B70" t="s">
-        <v>68</v>
-      </c>
       <c r="C70" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71">
         <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
+      <c r="B71" t="s">
         <v>70</v>
       </c>
-      <c r="B71" t="s">
-        <v>69</v>
-      </c>
       <c r="C71" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72">
         <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="B72" t="s">
         <v>71</v>
       </c>
-      <c r="B72" t="s">
-        <v>70</v>
-      </c>
       <c r="C72" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73">
         <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+      <c r="B73" t="s">
         <v>72</v>
       </c>
-      <c r="B73" t="s">
-        <v>71</v>
-      </c>
       <c r="C73" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74">
         <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="B74" t="s">
         <v>73</v>
       </c>
-      <c r="B74" t="s">
-        <v>72</v>
-      </c>
       <c r="C74" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75">
         <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="B75" t="s">
         <v>74</v>
       </c>
-      <c r="B75" t="s">
-        <v>73</v>
-      </c>
       <c r="C75" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76">
         <f t="shared" si="1"/>
+        <v>76</v>
+      </c>
+      <c r="B76" t="s">
         <v>75</v>
       </c>
-      <c r="B76" t="s">
-        <v>74</v>
-      </c>
       <c r="C76" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77">
         <f t="shared" si="1"/>
+        <v>77</v>
+      </c>
+      <c r="B77" t="s">
         <v>76</v>
       </c>
-      <c r="B77" t="s">
-        <v>75</v>
-      </c>
       <c r="C77" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78">
         <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+      <c r="B78" t="s">
         <v>77</v>
       </c>
-      <c r="B78" t="s">
-        <v>76</v>
-      </c>
       <c r="C78" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79">
         <f t="shared" si="1"/>
+        <v>79</v>
+      </c>
+      <c r="B79" t="s">
         <v>78</v>
       </c>
-      <c r="B79" t="s">
-        <v>77</v>
-      </c>
       <c r="C79" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80">
         <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="B80" t="s">
         <v>79</v>
       </c>
-      <c r="B80" t="s">
-        <v>78</v>
-      </c>
       <c r="C80" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81">
         <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
+      <c r="B81" t="s">
         <v>80</v>
       </c>
-      <c r="B81" t="s">
-        <v>79</v>
-      </c>
       <c r="C81" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82">
         <f t="shared" si="1"/>
+        <v>82</v>
+      </c>
+      <c r="B82" t="s">
         <v>81</v>
       </c>
-      <c r="B82" t="s">
-        <v>80</v>
-      </c>
       <c r="C82" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83">
         <f t="shared" si="1"/>
+        <v>83</v>
+      </c>
+      <c r="B83" t="s">
         <v>82</v>
       </c>
-      <c r="B83" t="s">
-        <v>81</v>
-      </c>
       <c r="C83" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84">
         <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+      <c r="B84" t="s">
         <v>83</v>
       </c>
-      <c r="B84" t="s">
-        <v>82</v>
-      </c>
       <c r="C84" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85">
         <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+      <c r="B85" t="s">
         <v>84</v>
       </c>
-      <c r="B85" t="s">
-        <v>83</v>
-      </c>
       <c r="C85" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86">
         <f t="shared" si="1"/>
+        <v>86</v>
+      </c>
+      <c r="B86" t="s">
         <v>85</v>
       </c>
-      <c r="B86" t="s">
-        <v>84</v>
-      </c>
       <c r="C86" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87">
         <f t="shared" si="1"/>
+        <v>87</v>
+      </c>
+      <c r="B87" t="s">
         <v>86</v>
       </c>
-      <c r="B87" t="s">
-        <v>85</v>
-      </c>
       <c r="C87" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88">
         <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="B88" t="s">
         <v>87</v>
       </c>
-      <c r="B88" t="s">
-        <v>86</v>
-      </c>
       <c r="C88" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89">
         <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+      <c r="B89" t="s">
         <v>88</v>
       </c>
-      <c r="B89" t="s">
-        <v>87</v>
-      </c>
       <c r="C89" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90">
         <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="B90" t="s">
         <v>89</v>
       </c>
-      <c r="B90" t="s">
-        <v>88</v>
-      </c>
       <c r="C90" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91">
         <f t="shared" si="1"/>
+        <v>91</v>
+      </c>
+      <c r="B91" t="s">
         <v>90</v>
       </c>
-      <c r="B91" t="s">
-        <v>89</v>
-      </c>
       <c r="C91" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92">
         <f t="shared" si="1"/>
+        <v>92</v>
+      </c>
+      <c r="B92" t="s">
         <v>91</v>
       </c>
-      <c r="B92" t="s">
-        <v>90</v>
-      </c>
       <c r="C92" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93">
         <f t="shared" si="1"/>
+        <v>93</v>
+      </c>
+      <c r="B93" t="s">
         <v>92</v>
       </c>
-      <c r="B93" t="s">
-        <v>91</v>
-      </c>
       <c r="C93" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94">
         <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+      <c r="B94" t="s">
         <v>93</v>
       </c>
-      <c r="B94" t="s">
-        <v>92</v>
-      </c>
       <c r="C94" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95">
         <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="B95" t="s">
         <v>94</v>
       </c>
-      <c r="B95" t="s">
-        <v>93</v>
-      </c>
       <c r="C95" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96">
         <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+      <c r="B96" t="s">
         <v>95</v>
       </c>
-      <c r="B96" t="s">
-        <v>94</v>
-      </c>
       <c r="C96" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97">
         <f t="shared" si="1"/>
+        <v>97</v>
+      </c>
+      <c r="B97" t="s">
         <v>96</v>
       </c>
-      <c r="B97" t="s">
-        <v>95</v>
-      </c>
       <c r="C97" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98">
         <f t="shared" si="1"/>
+        <v>98</v>
+      </c>
+      <c r="B98" t="s">
         <v>97</v>
       </c>
-      <c r="B98" t="s">
-        <v>96</v>
-      </c>
       <c r="C98" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99">
         <f t="shared" si="1"/>
+        <v>99</v>
+      </c>
+      <c r="B99" t="s">
         <v>98</v>
       </c>
-      <c r="B99" t="s">
-        <v>97</v>
-      </c>
       <c r="C99" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100">
         <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="B100" t="s">
         <v>99</v>
       </c>
-      <c r="B100" t="s">
-        <v>98</v>
-      </c>
       <c r="C100" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101">
         <f t="shared" si="1"/>
+        <v>101</v>
+      </c>
+      <c r="B101" t="s">
         <v>100</v>
       </c>
-      <c r="B101" t="s">
-        <v>99</v>
-      </c>
       <c r="C101" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102">
         <f t="shared" si="1"/>
+        <v>102</v>
+      </c>
+      <c r="B102" t="s">
         <v>101</v>
       </c>
-      <c r="B102" t="s">
-        <v>100</v>
-      </c>
       <c r="C102" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103">
         <f t="shared" si="1"/>
+        <v>103</v>
+      </c>
+      <c r="B103" t="s">
         <v>102</v>
       </c>
-      <c r="B103" t="s">
-        <v>101</v>
-      </c>
       <c r="C103" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104">
         <f t="shared" si="1"/>
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B104" t="s">
-        <v>102</v>
+        <v>206</v>
       </c>
       <c r="C104" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A105">
-        <f t="shared" si="1"/>
-        <v>104</v>
-      </c>
-      <c r="B105" t="s">
-        <v>208</v>
-      </c>
-      <c r="C105" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>